<commit_message>
created new md file for json linq
</commit_message>
<xml_diff>
--- a/UiPathlinqCodesCheetSheet.xlsx
+++ b/UiPathlinqCodesCheetSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitSpace\uipathLinq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\UiPathLinq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9596A489-7E49-4460-B350-F93AF7F35D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9AB6CC-4E20-422B-A5DC-B330931B1DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datatable" sheetId="1" r:id="rId1"/>
@@ -369,13 +369,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="50.90625" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -383,7 +383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -402,7 +402,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -412,9 +412,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D39D134-4246-43BC-99E0-BA955C659A0B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>